<commit_message>
Traffic fines dataset updated
some minor corrections
</commit_message>
<xml_diff>
--- a/input/TrafficFinesDataset.xlsx
+++ b/input/TrafficFinesDataset.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adeladelrio/Trabajo/Research/ppibot/icpm 2022 paper/additionalMaterial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2F024B-F525-6046-853B-9102797507C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6241CD4-080E-2D4E-AA1E-A5F9BD584066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1740" windowWidth="27640" windowHeight="16300" xr2:uid="{D18CD79D-57ED-C247-8D36-08BA5FB25249}"/>
+    <workbookView xWindow="880" yWindow="5840" windowWidth="27640" windowHeight="16300" xr2:uid="{D18CD79D-57ED-C247-8D36-08BA5FB25249}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
-  <si>
-    <t>PPI definition</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>Reason to exclude it</t>
   </si>
@@ -336,10 +333,59 @@
     <t xml:space="preserve">#  ambiguous information </t>
   </si>
   <si>
-    <t>Legend</t>
-  </si>
-  <si>
     <t>Total amount of dismissed fines should go down for 30 percent</t>
+  </si>
+  <si>
+    <t>PPI description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend: </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> those PPIs for which the creation of a goldstandard was not possible </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>green</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> those for which a goldstandard was defined manually</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -827,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7A37BC-F705-1E47-9553-78100BA001FC}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -839,395 +885,401 @@
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="34">
+      <c r="A11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="34">
-      <c r="A11" s="7" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4" t="s">
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="51">
+      <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="68">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="34">
+      <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="34">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17">
+      <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="34">
       <c r="A18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="34">
       <c r="A21" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="8"/>
     </row>
     <row r="25" spans="1:2" ht="17">
       <c r="A25" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" ht="17">
       <c r="A29" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17">
       <c r="A30" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17">
       <c r="A31" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17">
       <c r="A33" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17">
       <c r="A34" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17">
       <c r="A35" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17">
       <c r="A37" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17">
       <c r="A39" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="34">
       <c r="A40" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="34">
       <c r="A41" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42" s="3"/>
     </row>
     <row r="43" spans="1:2" ht="34">
       <c r="A43" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17">
       <c r="A46" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17">
       <c r="A47" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="31">
       <c r="A50" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="34">
       <c r="A53" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="34">
       <c r="A54" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="16">
         <f>COUNTIF(B2:B54,"information not available in the log")</f>
@@ -1236,7 +1288,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" s="16">
         <f>COUNTIF(B2:B54,"not supported by our approach")</f>
@@ -1245,7 +1297,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" s="16">
         <f>COUNTIF(B2:B54,"not supported by PPINOT")</f>
@@ -1254,7 +1306,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" s="16">
         <f>COUNTIF(B2:B54,"ambiguous information")</f>

</xml_diff>